<commit_message>
remove duplicates from list of unmatched persons
</commit_message>
<xml_diff>
--- a/unmatched_persons.xlsx
+++ b/unmatched_persons.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdewey/Development/code/84000-data-rdf/xml-parsing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DAAEAA4-4F2C-604B-A5CC-A492D62003E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454564B4-FEA6-1942-A446-A7A9E85C734C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{EC367144-908E-504C-8C8B-401A89C276C2}"/>
+    <workbookView xWindow="11760" yWindow="500" windowWidth="16660" windowHeight="16080" xr2:uid="{EC367144-908E-504C-8C8B-401A89C276C2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="unmatched_persons" localSheetId="0">Sheet1!$A$1:$D$4</definedName>
+    <definedName name="unmatched_persons" localSheetId="0">Sheet3!$A$1:$D$43</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{CAB1A5FF-9FE0-CD41-BDB2-C00A4726233B}" name="unmatched_persons" type="6" refreshedVersion="7" background="1" saveData="1">
+  <connection id="1" xr16:uid="{545B8941-DF37-024D-ADF6-E491B0610223}" name="unmatched_persons" type="6" refreshedVersion="7" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="/Users/williamdewey/Development/code/84000-data-rdf/xml-parsing/unmatched_persons.csv" tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>84000 ID</t>
   </si>
@@ -78,10 +78,367 @@
     <t>vidyakaraprabha</t>
   </si>
   <si>
-    <t>eft:bidyakaraprabha</t>
-  </si>
-  <si>
-    <t>bidyakaraprabha</t>
+    <t>eft:palgyi-lh-npo</t>
+  </si>
+  <si>
+    <t>Palgyi Lhünpo</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>eft:paltsek</t>
+  </si>
+  <si>
+    <t>Paltsek</t>
+  </si>
+  <si>
+    <t>{'P8211': ['rgya gar gyi mkhan po bid+yA ka ra pra b+ha', 'bid+yA ka ra pra b+hA/', 'vidyākaraprabha'], nan: ['d+har+m+ma shrI pra b+ha'], 'P4258': ["lots+tsha ba ban de dpal 'byor", "dpal 'byor/"]}</t>
+  </si>
+  <si>
+    <t>eft:dharmasribhadra</t>
+  </si>
+  <si>
+    <t>eft:jinamitra</t>
+  </si>
+  <si>
+    <t>Jinamitra</t>
+  </si>
+  <si>
+    <t>{'P8205': ['zhu chen gyi lots+tsha ba ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:yesh-d-</t>
+  </si>
+  <si>
+    <t>Yeshé Dé</t>
+  </si>
+  <si>
+    <t>eft:sakyasena</t>
+  </si>
+  <si>
+    <t>sakyasena</t>
+  </si>
+  <si>
+    <t>{'P8213': ['rgya gar gyi mkhan po bid+yA ka ra sing ha', 'bIr+ya ka ra sing+ha/', 'vīryakarasiṁha,vīryasiṁha'], 'P8182': ['zhu chen gyi lots+tsha ba ban de dpal brtsegs', 'ka ba dpal brtsegs/']}</t>
+  </si>
+  <si>
+    <t>eft:jnanasiddhi</t>
+  </si>
+  <si>
+    <t>jnanasiddhi</t>
+  </si>
+  <si>
+    <t>eft:dharmatasila</t>
+  </si>
+  <si>
+    <t>eft:dipamkarasrijnana</t>
+  </si>
+  <si>
+    <t>{'P1KG8854': ['rgya gar gyi mkhan po shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'], 'P8209': ['dzi na mi tra', 'slob dpon dzi na mi tra/', 'jinamitra'], 'P8205': ['zhu chen gyi lots+tsha ba ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:anandasri-s-</t>
+  </si>
+  <si>
+    <t>anandasri (s)</t>
+  </si>
+  <si>
+    <t>{'P2147': ["lo ts+tsha ba shAkya'i dge slong nyi ma rgyal mtshan", 'nyi ma rgyal mtshan/'], nan: ['gtsug lag khang chen po dpal thar pa gling du bsgyur cing zhus te gtan la phab pa']}</t>
+  </si>
+  <si>
+    <t>eft:kawa-paltsek-under-the-name-paltsek-raksita-</t>
+  </si>
+  <si>
+    <t>Kawa Paltsek (under the name Paltsek Rakṣita)</t>
+  </si>
+  <si>
+    <t>{'P8228': ['rgya gar gyi mkhan po su ren dra bo d+hi', 'lha dbang byang chub', 'surendrabodhi'], 'P8182': ['zhu chen gyi lo tsa ba ban de dpal brtsegs rak+Shi ta', 'ka ba dpal brtsegs/']}</t>
+  </si>
+  <si>
+    <t>{'P8209': ['rgya gar gyi mkhan po dzi na mi tra', 'slob dpon dzi na mi tra/', 'jinamitra'], 'P8228': ['su ren dra bo d+hi', 'lha dbang byang chub', 'surendrabodhi'], 'P8205': ['zhu chen gyi lo ts+tsha ba ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:band-yesh-d-</t>
+  </si>
+  <si>
+    <t>Bandé Yeshé Dé</t>
+  </si>
+  <si>
+    <t>eft:danasila</t>
+  </si>
+  <si>
+    <t>Danaśila</t>
+  </si>
+  <si>
+    <t>{'P8209': ['rgya gar gyi mkhan po dzi na mi tra', 'slob dpon dzi na mi tra/', 'jinamitra'], 'P3214': ['dA na shI la', 'dA na shI la/', 'dānaśīla'], 'P8205': ['zhu chen gyi lots+tsha ba ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:t-vidyakarasimha</t>
+  </si>
+  <si>
+    <t>t. Vidyākarasiṃha</t>
+  </si>
+  <si>
+    <t>{'P8213': ['rgya gar gyi mkhan po bid+yA ka ra sing ha', 'bIr+ya ka ra sing+ha/', 'vīryakarasiṁha,vīryasiṁha'], 'P8260': ['lots+tsha ba ban de dpal gyi dbyangs', 'dpal dbyangs/'], 'P8182': ['zhu chen gyi lots+tsha ba ban de dpal brtsegs', 'ka ba dpal brtsegs/']}</t>
+  </si>
+  <si>
+    <t>{'P8228': ['rgya gar gyi mkhan po su ren dra bo d+hi', 'lha dbang byang chub', 'surendrabodhi'], 'P8205': ['zhu chen gyi lots+tsha ba ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:yesh-nyingpo</t>
+  </si>
+  <si>
+    <t>Yeshé Nyingpo</t>
+  </si>
+  <si>
+    <t>{'P2548': ['rgya gar gyi mkhan po pradz+nyA bar ma', 'shes rab go cha/', 'prajñāvarman'], 'P4255': ['lots+tsha ba ban de ye shes snying po', 'ye shes snying po/'], 'P8182': ['zhu chen gyi lots+tsha ba ban de dpal brtsegs', 'ka ba dpal brtsegs/']}</t>
+  </si>
+  <si>
+    <t>eft:leki-d-</t>
+  </si>
+  <si>
+    <t>Leki Dé</t>
+  </si>
+  <si>
+    <t>{'P2548': ['rgya gar gyi mkhan po pradz+nyA warma', 'shes rab go cha/', 'prajñāvarman'], 'P8263': ['lo ts+tsha ba ban de legs kyi sde', 'legs kyi sde/'], 'P8205': ['zhu chen gyi lo ts+tsha ba ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:surendrabodhi</t>
+  </si>
+  <si>
+    <t>Surendrabodhi</t>
+  </si>
+  <si>
+    <t>{'P8209': ['rgya gar gyi mkhan po dzi na mi tra', 'slob dpon dzi na mi tra/', 'jinamitra'], 'P1KG8854': ['shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'], 'P8205': ['zhu chen gyi lots+tsha ba _ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:yesh-d-ye-shes-sde-</t>
+  </si>
+  <si>
+    <t>Yeshé Dé (ye shes sde)</t>
+  </si>
+  <si>
+    <t>{'P3214': ['rgya gar gyi mkhan po dA na shI la', 'dA na shI la/', 'dānaśīla'], 'P8205': ['zhu chen gyi lo tsA ba _ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:srilendrabodhi</t>
+  </si>
+  <si>
+    <t>Śrīlendrabodhi</t>
+  </si>
+  <si>
+    <t>{'P1KG8854': ['rgya gar gyi mkhan po shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'], 'P8266': ['zhu chen gyi lots+tsha ba ban de d+harma tA shI la', 'chos nyid tshul khrims', 'Dharmatāśīla']}</t>
+  </si>
+  <si>
+    <t>eft:silendrabodhi</t>
+  </si>
+  <si>
+    <t>Śilendrabodhi</t>
+  </si>
+  <si>
+    <t>{'P8205': ['zhu chen gyi lo ts+tsha ba ban+de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>Dīpaṃkaraśrījñāna</t>
+  </si>
+  <si>
+    <t>{'P3379': ['rgya gar gyi mkhan po dI paM ka ra shrI dz+nyA na', 'a ti sha', 'dīpaṁkaraśrijñāna,atīśa'], 'P1242': ["lo ts+tsha ba dge slong dge ba'i blo gros", "dge ba'i blo gros/"]}</t>
+  </si>
+  <si>
+    <t>eft:buddhaprabha</t>
+  </si>
+  <si>
+    <t>Buddhaprabha</t>
+  </si>
+  <si>
+    <t>{'P8209': ['rgya gar gyi mkhan po dzi na mi tra', 'slob dpon dzi na mi tra/', 'jinamitra'], 'P3214': ['dA na shI la', 'dA na shI la/', 'dānaśīla'], 'P8268': ['bud d+ha pra b+ha'], 'P8205': ['zhu chen gyi lots+tsha ba ban+de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:prajnavarma</t>
+  </si>
+  <si>
+    <t>prajnavarma</t>
+  </si>
+  <si>
+    <t>{'P8209': ['rgya gar gyi mkhan po dzi na mi tra', 'slob dpon dzi na mi tra/', 'jinamitra'], nan: ['pradz+nyA bad+ma'], 'P8205': ['zhu chen gyi lo ts+tsha ba ban+de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:dharmapala</t>
+  </si>
+  <si>
+    <t>Dharmapāla</t>
+  </si>
+  <si>
+    <t>{'P4CZ16819': ['rgya gar gyi mkhan po shAkya pra b+ha', "shAkya 'od/", "shAkya 'od/", 'śākyaprabha'], 'P0RK8': ['d+harma pA la', 'dpal ldan chos skyong /'], 'P8209': ['dzi na mi tra', 'slob dpon dzi na mi tra/', 'jinamitra'], 'P8266': ['zhu chen gyi lo tsA ba ban+de d+harma tA shI la', 'chos nyid tshul khrims', 'Dharmatāśīla']}</t>
+  </si>
+  <si>
+    <t>eft:t-jnanagarbha</t>
+  </si>
+  <si>
+    <t>t. Jñānagarbha</t>
+  </si>
+  <si>
+    <t>{'P8217': ['rgya gar gyi mkhan po dz+nyA na gar b+ha', 'dz+nyA na gar b+ha/', 'jñānagarbha ?'], 'P4255': ['lots+tsha ba ban+de ye shes snying po', 'ye shes snying po/'], 'P8182': ['zhus chen gyi lots+tsha ba ban+de dpal brtsegs', 'ka ba dpal brtsegs/']}</t>
+  </si>
+  <si>
+    <t>eft:vidyakarasimha</t>
+  </si>
+  <si>
+    <t>Vidyākarasiṃha</t>
+  </si>
+  <si>
+    <t>{'P8219': ['rgya gar gyi mkhan po bi shud+d+ha sing ha', 'bi shud+d+ha sing ha/', 'viśuddhasiṃha'], 'P4263': ['lots+tsha ba ban+de dge ba dpal', 'dge ba dpal'], 'P8220': ['zhu chen gyi lots+tsha ba ban+de de ba tsan dra', 'devacandra']}</t>
+  </si>
+  <si>
+    <t>Dharmatāśila</t>
+  </si>
+  <si>
+    <t>{'P8266': ['zhu chen gyi lots+tsha ba ban de d+harma tA shI las zhus', 'chos nyid tshul khrims', 'Dharmatāśīla']}</t>
+  </si>
+  <si>
+    <t>eft:ch-nyi-tsultrim</t>
+  </si>
+  <si>
+    <t>Chönyi Tsultrim</t>
+  </si>
+  <si>
+    <t>{'P8266': ['lo ts+tsha ba ban de chos nyid tshul khrims', 'chos nyid tshul khrims', 'Dharmatāśīla']}</t>
+  </si>
+  <si>
+    <t>eft:jnanasidhi</t>
+  </si>
+  <si>
+    <t>jnanasidhi</t>
+  </si>
+  <si>
+    <t>{'P8209': ['rgya gar gyi mkhan po dzi na mi tra', 'slob dpon dzi na mi tra/', 'jinamitra'], 'P8222': ['dz+nyA na sid+d+hi', 'dz+nyA na sid+dhi/', 'jñānasiddhi'], 'P8205': ['zhu chen gyi lo ts+tsha ba ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>{'P00KG07267': ['rgya gar gyi mkhan po sarba dz+nya de ba', 'sarba dz+nyA de ba/', 'sarvajñādeva'], 'P8182': ['zhu chen gyi lo ts+tsha ba ban de dpal brtsegs', 'ka ba dpal brtsegs/']}</t>
+  </si>
+  <si>
+    <t>eft:rinchen-tso</t>
+  </si>
+  <si>
+    <t>Rinchen Tso</t>
+  </si>
+  <si>
+    <t>{'P8273': ["lo ts+tsha ba ban de rin chen 'tsho", "rin chen 'tsho/"], 'P8266': ['chos nyid tshul khrims', 'chos nyid tshul khrims', 'Dharmatāśīla']}</t>
+  </si>
+  <si>
+    <t>eft:manjusrigarbha</t>
+  </si>
+  <si>
+    <t>Mañjuśrīgarbha</t>
+  </si>
+  <si>
+    <t>{'P4CZ16780': ['rgya gar gyi mkhan po many+dzu shrI gar+b+ha', 'many+dzu shrI gar+b+ha/', 'majuśrīgarbha'], 'P8267': ['bi dza ya shI la'], 'P1KG8854': ['shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'], 'P8205': ['zhu chen gyi lo ts+tsha ba ban de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:rnam-par-mi-rtog-pa</t>
+  </si>
+  <si>
+    <t>rnam par mi rtog pa</t>
+  </si>
+  <si>
+    <t>{'P0TMP080': ["rgya'i mkhan po hwa shang zab mo", 'hwa shang zab mo'], nan: ['zhu chen gyi lo tsa ba ban de rnam par mi rtog']}</t>
+  </si>
+  <si>
+    <t>eft:siladharma</t>
+  </si>
+  <si>
+    <t>siladharma</t>
+  </si>
+  <si>
+    <t>{nan: ["rgya gar gyi d+harma rgya'i yi ge las ban de rnam par mi rtog"]}</t>
+  </si>
+  <si>
+    <t>eft:zhang-yesh-d-</t>
+  </si>
+  <si>
+    <t>Zhang Yeshé Dé</t>
+  </si>
+  <si>
+    <t>{'P8228': ['rgya gar gyi mkhan po su ren dra bo d+hi', 'lha dbang byang chub', 'surendrabodhi'], 'P8205': ['zhu chen gyi lo ts+tsha ba ban de zhang ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>Dharmaśrībhadra</t>
+  </si>
+  <si>
+    <t>{nan: ['rgya gar gyi mkhan po d+harmA shrI b+ha dra'], 'P4242': ['zhu chen gyi lots+tsha ba dge slong shes rab legs pa', 'shes rab legs pa/'], 'P753': ['sgra bsgyur gyi lots+tsha ba chen po dge slong rin chen bzang po', 'rin chen bzang po/']}</t>
+  </si>
+  <si>
+    <t>eft:sakya-yesh-</t>
+  </si>
+  <si>
+    <t>Śākya Yeshé</t>
+  </si>
+  <si>
+    <t>{'P8151': ['paN+Di ta ga ye d+ha ra', 'ga ya dha ra/', 'gayādhara'], 'P3285': ['lots+tsha ba dge slong shAkya ye shes', 'shAkya ye shes/']}</t>
+  </si>
+  <si>
+    <t>eft:jinavara</t>
+  </si>
+  <si>
+    <t>Jinavara</t>
+  </si>
+  <si>
+    <t>{nan: ["bod kyi lo ts+tsha ba chen po 'gos lhas btsas"]}</t>
+  </si>
+  <si>
+    <t>eft:trakpa-gyaltsen</t>
+  </si>
+  <si>
+    <t>Trakpa Gyaltsen</t>
+  </si>
+  <si>
+    <t>{'P4CZ10553': ['paN+Di ta rat+na shrI', 'rin chen dpal ye shes/', 'ratnaśrījñāna ?'], 'P2637': ['lo ts+tsha ba grags pa rgyal mtshan', 'grags pa rgyal mtshan/'], nan: ["dpal ldan sa skya'i gtsug lag khang chen po"]}</t>
+  </si>
+  <si>
+    <t>eft:phakpa-sherab</t>
+  </si>
+  <si>
+    <t>Phakpa Sherab</t>
+  </si>
+  <si>
+    <t>{'P8206': ["kha che'i paN+Di ta tse lu", 'celu-pa'], 'P3709': ["bod kyi lo ts+tsha ba 'phags pa shes rab", 'phags pa shes rab/']}</t>
+  </si>
+  <si>
+    <t>{'P8209': ['rgya gar gyi mkhan po dzi na mi tra', 'slob dpon dzi na mi tra/', 'jinamitra'], 'P3214': ['dA na shI la', 'dA na shI la/', 'dānaśīla'], 'P8205': ['zhu chen gyi lots+tsha ba ban+de ye shes sde', 'ye shes sde/']}</t>
+  </si>
+  <si>
+    <t>eft:kumarakalasa</t>
+  </si>
+  <si>
+    <t>Kumārakalaśa</t>
+  </si>
+  <si>
+    <t>{'P4CZ15137': ['rgya gar gyi mkhan po dge bsnyen chen po ku mA ra ka la sha', 'gzhon nu bum pa/', 'kumārakalasa'], 'P8216': ['sgra sgyur gyi lots+tsha ba dge slong shAkya blo gros', 'shAkya blo gros/']}</t>
+  </si>
+  <si>
+    <t>eft:dipamkara-srijnana</t>
+  </si>
+  <si>
+    <t>Dīpaṃkara Śrījñāna</t>
+  </si>
+  <si>
+    <t>{'P3379': ['rgya gar gyi mkhan po chen po dI paM ka ra shrIdz+nyA na', 'a ti sha', 'dīpaṁkaraśrijñāna,atīśa'], 'P1242': ["lots+tsha ba dge slong dge ba'i blo gros", "dge ba'i blo gros/"], 'P3456': ['dge slong tshul khrims rgyal ba', 'tshul khrims rgyal ba/']}</t>
+  </si>
+  <si>
+    <t>eft:band-yesh-de</t>
+  </si>
+  <si>
+    <t>Bandé Yeshé De</t>
+  </si>
+  <si>
+    <t>eft:buddhakaravarma</t>
+  </si>
+  <si>
+    <t>Buddhākaravarma</t>
+  </si>
+  <si>
+    <t>{nan: ['rgya gar gyi mkhan po bud+d+ha A ka ra ba rma'], 'P3890': ['lo ts+tsha ba dge slong chos kyi shes rab', 'chos kyi shes rab/']}</t>
   </si>
 </sst>
 </file>
@@ -137,7 +494,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="unmatched_persons" connectionId="1" xr16:uid="{9C7F7846-BDF8-1044-B0D6-61BFD152290F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="unmatched_persons" connectionId="1" xr16:uid="{9481A802-E26D-7E42-B51A-A276B8AE3077}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -436,16 +793,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676823D4-EB45-6B44-898D-B240ECF9F6EF}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4AEDBC-06FA-F54B-8B31-55BADC9046FA}">
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="80.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -465,13 +822,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -479,10 +836,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -493,13 +850,559 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more data files, and test data uploading
</commit_message>
<xml_diff>
--- a/unmatched_persons.xlsx
+++ b/unmatched_persons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdewey/Development/code/84000-data-rdf/xml-parsing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454564B4-FEA6-1942-A446-A7A9E85C734C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396A76D5-53BB-F14E-84F6-8774C3178A82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11760" yWindow="500" windowWidth="16660" windowHeight="16080" xr2:uid="{EC367144-908E-504C-8C8B-401A89C276C2}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28400" windowHeight="16020" xr2:uid="{EC367144-908E-504C-8C8B-401A89C276C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -454,12 +454,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -474,8 +480,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,7 +803,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4AEDBC-06FA-F54B-8B31-55BADC9046FA}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="A5:C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -859,17 +868,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>